<commit_message>
Changes to support parallel processing.
</commit_message>
<xml_diff>
--- a/Support/configDescriptions.xlsx
+++ b/Support/configDescriptions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\RemotelyBackedUp\Git\StepTextConversion\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7CAF23-A6BC-40D5-A733-AB2B8D978801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D393189-D540-4452-AD32-D3EC17CA3CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{128561E6-B5C2-46ED-B2EC-132D38FABE72}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="PatternBasedElements" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IndividualElements!$A$2:$I$175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IndividualElements!$A$2:$I$176</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="361">
   <si>
     <t>stepDbgAddDebugAttributesToNodes</t>
   </si>
@@ -1104,6 +1104,15 @@
   </si>
   <si>
     <t>May occur multiple times.  Lines should be of the form 'stepPreprocessingRegexWhenNotStartingFromOsis=regex=&gt;replacement'.  Each statement defines a modification to be applied to the input data before processing.</t>
+  </si>
+  <si>
+    <t>stepPermitParallelRunning</t>
+  </si>
+  <si>
+    <t>Says whether to permit parallel running where the processing can use it.  May, for instance, be useful to turn it off when debugging.</t>
+  </si>
+  <si>
+    <t>Anywhere</t>
   </si>
 </sst>
 </file>
@@ -1876,13 +1885,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACFB32A-97A1-4D27-B533-EB469205C671}">
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B99" sqref="B99"/>
+      <selection pane="bottomRight" activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4306,51 +4315,48 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>63</v>
+        <v>358</v>
       </c>
       <c r="B101" t="s">
-        <v>190</v>
+        <v>359</v>
       </c>
       <c r="C101" t="s">
         <v>27</v>
       </c>
       <c r="D101" t="s">
-        <v>191</v>
+        <v>24</v>
       </c>
       <c r="E101" t="s">
-        <v>192</v>
+        <v>101</v>
       </c>
       <c r="F101" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="G101" t="s">
-        <v>225</v>
+        <v>360</v>
       </c>
       <c r="H101" t="s">
-        <v>318</v>
-      </c>
-      <c r="I101" t="s">
-        <v>227</v>
+        <v>322</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B102" t="s">
-        <v>151</v>
+        <v>190</v>
       </c>
       <c r="C102" t="s">
         <v>27</v>
       </c>
       <c r="D102" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="E102" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="F102" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="G102" t="s">
         <v>225</v>
@@ -4359,15 +4365,15 @@
         <v>318</v>
       </c>
       <c r="I102" t="s">
-        <v>316</v>
+        <v>227</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B103" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="C103" t="s">
         <v>27</v>
@@ -4376,7 +4382,7 @@
         <v>166</v>
       </c>
       <c r="E103" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="F103" t="s">
         <v>200</v>
@@ -4388,33 +4394,36 @@
         <v>318</v>
       </c>
       <c r="I103" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>84</v>
+      </c>
+      <c r="B104" t="s">
+        <v>111</v>
+      </c>
+      <c r="C104" t="s">
+        <v>27</v>
+      </c>
+      <c r="D104" t="s">
+        <v>166</v>
+      </c>
+      <c r="E104" t="s">
+        <v>101</v>
+      </c>
+      <c r="F104" t="s">
+        <v>200</v>
+      </c>
+      <c r="G104" t="s">
+        <v>225</v>
+      </c>
+      <c r="H104" t="s">
+        <v>318</v>
+      </c>
+      <c r="I104" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>316</v>
-      </c>
-      <c r="C104" t="s">
-        <v>316</v>
-      </c>
-      <c r="D104" t="s">
-        <v>316</v>
-      </c>
-      <c r="E104" t="s">
-        <v>316</v>
-      </c>
-      <c r="F104" t="s">
-        <v>316</v>
-      </c>
-      <c r="G104" t="s">
-        <v>316</v>
-      </c>
-      <c r="H104" t="s">
-        <v>316</v>
-      </c>
-      <c r="I104" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4444,9 +4453,6 @@
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>308</v>
-      </c>
       <c r="B106" t="s">
         <v>316</v>
       </c>
@@ -4474,28 +4480,28 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>37</v>
+        <v>308</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>316</v>
       </c>
       <c r="C107" t="s">
-        <v>27</v>
+        <v>316</v>
       </c>
       <c r="D107" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="E107" t="s">
-        <v>124</v>
+        <v>316</v>
       </c>
       <c r="F107" t="s">
-        <v>200</v>
+        <v>316</v>
       </c>
       <c r="G107" t="s">
-        <v>225</v>
+        <v>316</v>
       </c>
       <c r="H107" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I107" t="s">
         <v>316</v>
@@ -4503,10 +4509,10 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B108" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C108" t="s">
         <v>27</v>
@@ -4524,33 +4530,36 @@
         <v>225</v>
       </c>
       <c r="H108" t="s">
+        <v>318</v>
+      </c>
+      <c r="I108" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>38</v>
+      </c>
+      <c r="B109" t="s">
+        <v>129</v>
+      </c>
+      <c r="C109" t="s">
+        <v>27</v>
+      </c>
+      <c r="D109" t="s">
+        <v>24</v>
+      </c>
+      <c r="E109" t="s">
+        <v>124</v>
+      </c>
+      <c r="F109" t="s">
+        <v>200</v>
+      </c>
+      <c r="G109" t="s">
+        <v>225</v>
+      </c>
+      <c r="H109" t="s">
         <v>330</v>
-      </c>
-      <c r="I108" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>316</v>
-      </c>
-      <c r="C109" t="s">
-        <v>316</v>
-      </c>
-      <c r="D109" t="s">
-        <v>316</v>
-      </c>
-      <c r="E109" t="s">
-        <v>316</v>
-      </c>
-      <c r="F109" t="s">
-        <v>316</v>
-      </c>
-      <c r="G109" t="s">
-        <v>316</v>
-      </c>
-      <c r="H109" t="s">
-        <v>316</v>
       </c>
       <c r="I109" t="s">
         <v>316</v>
@@ -4583,9 +4592,6 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>309</v>
-      </c>
       <c r="B111" t="s">
         <v>316</v>
       </c>
@@ -4613,106 +4619,109 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>342</v>
+        <v>309</v>
       </c>
       <c r="B112" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
       <c r="C112" t="s">
-        <v>27</v>
+        <v>316</v>
       </c>
       <c r="D112" t="s">
-        <v>166</v>
+        <v>316</v>
       </c>
       <c r="E112" t="s">
         <v>316</v>
       </c>
       <c r="F112" t="s">
-        <v>202</v>
+        <v>316</v>
       </c>
       <c r="G112" t="s">
-        <v>223</v>
+        <v>316</v>
       </c>
       <c r="H112" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="I112" t="s">
-        <v>135</v>
+        <v>316</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B113" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C113" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D113" t="s">
-        <v>25</v>
+        <v>166</v>
+      </c>
+      <c r="E113" t="s">
+        <v>316</v>
       </c>
       <c r="F113" t="s">
-        <v>346</v>
+        <v>202</v>
       </c>
       <c r="G113" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="H113" t="s">
-        <v>25</v>
+        <v>323</v>
+      </c>
+      <c r="I113" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>344</v>
+      </c>
+      <c r="B114" t="s">
+        <v>345</v>
+      </c>
+      <c r="C114" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114" t="s">
+        <v>25</v>
+      </c>
+      <c r="F114" t="s">
+        <v>346</v>
+      </c>
+      <c r="G114" t="s">
+        <v>25</v>
+      </c>
+      <c r="H114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>337</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>224</v>
       </c>
-      <c r="C114" t="s">
-        <v>27</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="C115" t="s">
+        <v>27</v>
+      </c>
+      <c r="D115" t="s">
         <v>24</v>
       </c>
-      <c r="E114" t="s">
-        <v>316</v>
-      </c>
-      <c r="F114" t="s">
+      <c r="E115" t="s">
+        <v>316</v>
+      </c>
+      <c r="F115" t="s">
         <v>202</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G115" t="s">
         <v>223</v>
       </c>
-      <c r="H114" t="s">
+      <c r="H115" t="s">
         <v>327</v>
-      </c>
-      <c r="I114" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>316</v>
-      </c>
-      <c r="C115" t="s">
-        <v>316</v>
-      </c>
-      <c r="D115" t="s">
-        <v>316</v>
-      </c>
-      <c r="E115" t="s">
-        <v>316</v>
-      </c>
-      <c r="F115" t="s">
-        <v>316</v>
-      </c>
-      <c r="G115" t="s">
-        <v>316</v>
-      </c>
-      <c r="H115" t="s">
-        <v>316</v>
       </c>
       <c r="I115" t="s">
         <v>316</v>
@@ -4745,9 +4754,6 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>310</v>
-      </c>
       <c r="B117" t="s">
         <v>316</v>
       </c>
@@ -4775,28 +4781,28 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>3</v>
+        <v>310</v>
       </c>
       <c r="B118" t="s">
-        <v>154</v>
+        <v>316</v>
       </c>
       <c r="C118" t="s">
-        <v>27</v>
+        <v>316</v>
       </c>
       <c r="D118" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="E118" t="s">
         <v>316</v>
       </c>
       <c r="F118" t="s">
-        <v>204</v>
+        <v>316</v>
       </c>
       <c r="G118" t="s">
-        <v>225</v>
+        <v>316</v>
       </c>
       <c r="H118" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="I118" t="s">
         <v>316</v>
@@ -4804,10 +4810,10 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B119" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C119" t="s">
         <v>27</v>
@@ -4819,7 +4825,7 @@
         <v>316</v>
       </c>
       <c r="F119" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G119" t="s">
         <v>225</v>
@@ -4832,26 +4838,29 @@
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>2</v>
+      </c>
       <c r="B120" t="s">
-        <v>316</v>
+        <v>153</v>
       </c>
       <c r="C120" t="s">
-        <v>316</v>
+        <v>27</v>
       </c>
       <c r="D120" t="s">
-        <v>316</v>
+        <v>24</v>
       </c>
       <c r="E120" t="s">
         <v>316</v>
       </c>
       <c r="F120" t="s">
-        <v>316</v>
+        <v>205</v>
       </c>
       <c r="G120" t="s">
-        <v>316</v>
+        <v>225</v>
       </c>
       <c r="H120" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="I120" t="s">
         <v>316</v>
@@ -4884,9 +4893,6 @@
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>311</v>
-      </c>
       <c r="B122" t="s">
         <v>316</v>
       </c>
@@ -4914,28 +4920,28 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>18</v>
+        <v>311</v>
       </c>
       <c r="B123" t="s">
-        <v>161</v>
+        <v>316</v>
       </c>
       <c r="C123" t="s">
-        <v>27</v>
+        <v>316</v>
       </c>
       <c r="D123" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="E123" t="s">
-        <v>124</v>
+        <v>316</v>
       </c>
       <c r="F123" t="s">
-        <v>200</v>
+        <v>316</v>
       </c>
       <c r="G123" t="s">
-        <v>215</v>
+        <v>316</v>
       </c>
       <c r="H123" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I123" t="s">
         <v>316</v>
@@ -4943,10 +4949,10 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B124" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="C124" t="s">
         <v>27</v>
@@ -4972,10 +4978,10 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>340</v>
+        <v>19</v>
       </c>
       <c r="B125" t="s">
-        <v>339</v>
+        <v>193</v>
       </c>
       <c r="C125" t="s">
         <v>27</v>
@@ -4984,7 +4990,10 @@
         <v>24</v>
       </c>
       <c r="E125" t="s">
-        <v>341</v>
+        <v>124</v>
+      </c>
+      <c r="F125" t="s">
+        <v>200</v>
       </c>
       <c r="G125" t="s">
         <v>215</v>
@@ -4992,71 +5001,68 @@
       <c r="H125" t="s">
         <v>320</v>
       </c>
+      <c r="I125" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>268</v>
+        <v>340</v>
       </c>
       <c r="B126" t="s">
-        <v>220</v>
+        <v>339</v>
       </c>
       <c r="C126" t="s">
         <v>27</v>
       </c>
       <c r="D126" t="s">
-        <v>166</v>
+        <v>24</v>
       </c>
       <c r="E126" t="s">
-        <v>316</v>
-      </c>
-      <c r="F126" t="s">
-        <v>202</v>
+        <v>341</v>
       </c>
       <c r="G126" t="s">
         <v>215</v>
       </c>
       <c r="H126" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>268</v>
+      </c>
+      <c r="B127" t="s">
+        <v>220</v>
+      </c>
+      <c r="C127" t="s">
+        <v>27</v>
+      </c>
+      <c r="D127" t="s">
+        <v>166</v>
+      </c>
+      <c r="E127" t="s">
+        <v>316</v>
+      </c>
+      <c r="F127" t="s">
+        <v>202</v>
+      </c>
+      <c r="G127" t="s">
+        <v>215</v>
+      </c>
+      <c r="H127" t="s">
         <v>329</v>
       </c>
-      <c r="I126" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>180</v>
-      </c>
-      <c r="B128" t="s">
-        <v>207</v>
-      </c>
-      <c r="C128" t="s">
-        <v>27</v>
-      </c>
-      <c r="D128" t="s">
-        <v>24</v>
-      </c>
-      <c r="E128" t="s">
-        <v>160</v>
-      </c>
-      <c r="F128" t="s">
-        <v>199</v>
-      </c>
-      <c r="G128" t="s">
-        <v>215</v>
-      </c>
-      <c r="H128" t="s">
-        <v>320</v>
-      </c>
-      <c r="I128" t="s">
+      <c r="I127" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>70</v>
+        <v>180</v>
       </c>
       <c r="B129" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="C129" t="s">
         <v>27</v>
@@ -5065,7 +5071,7 @@
         <v>24</v>
       </c>
       <c r="E129" t="s">
-        <v>316</v>
+        <v>160</v>
       </c>
       <c r="F129" t="s">
         <v>199</v>
@@ -5082,28 +5088,28 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B130" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C130" t="s">
         <v>27</v>
       </c>
       <c r="D130" t="s">
-        <v>166</v>
+        <v>24</v>
       </c>
       <c r="E130" t="s">
-        <v>189</v>
+        <v>316</v>
       </c>
       <c r="F130" t="s">
         <v>199</v>
       </c>
       <c r="G130" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="H130" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="I130" t="s">
         <v>316</v>
@@ -5111,48 +5117,51 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="B131" t="s">
-        <v>109</v>
+        <v>188</v>
       </c>
       <c r="C131" t="s">
         <v>27</v>
       </c>
       <c r="D131" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="E131" t="s">
-        <v>25</v>
+        <v>189</v>
       </c>
       <c r="F131" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="G131" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="H131" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="I131" t="s">
-        <v>110</v>
+        <v>316</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>347</v>
+        <v>20</v>
       </c>
       <c r="B132" t="s">
-        <v>348</v>
+        <v>109</v>
       </c>
       <c r="C132" t="s">
         <v>27</v>
       </c>
       <c r="D132" t="s">
-        <v>24</v>
+        <v>191</v>
+      </c>
+      <c r="E132" t="s">
+        <v>25</v>
       </c>
       <c r="F132" t="s">
-        <v>349</v>
+        <v>212</v>
       </c>
       <c r="G132" t="s">
         <v>215</v>
@@ -5161,15 +5170,15 @@
         <v>320</v>
       </c>
       <c r="I132" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="B133" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="C133" t="s">
         <v>27</v>
@@ -5177,8 +5186,8 @@
       <c r="D133" t="s">
         <v>24</v>
       </c>
-      <c r="E133" t="s">
-        <v>341</v>
+      <c r="F133" t="s">
+        <v>349</v>
       </c>
       <c r="G133" t="s">
         <v>215</v>
@@ -5186,31 +5195,31 @@
       <c r="H133" t="s">
         <v>320</v>
       </c>
+      <c r="I133" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>338</v>
+      </c>
       <c r="B134" t="s">
-        <v>316</v>
+        <v>339</v>
       </c>
       <c r="C134" t="s">
-        <v>316</v>
+        <v>27</v>
       </c>
       <c r="D134" t="s">
-        <v>316</v>
+        <v>24</v>
       </c>
       <c r="E134" t="s">
-        <v>316</v>
-      </c>
-      <c r="F134" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="G134" t="s">
-        <v>316</v>
+        <v>215</v>
       </c>
       <c r="H134" t="s">
-        <v>316</v>
-      </c>
-      <c r="I134" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5240,9 +5249,6 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>312</v>
-      </c>
       <c r="B136" t="s">
         <v>316</v>
       </c>
@@ -5270,39 +5276,39 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>94</v>
+        <v>312</v>
       </c>
       <c r="B137" t="s">
-        <v>95</v>
+        <v>316</v>
       </c>
       <c r="C137" t="s">
-        <v>27</v>
+        <v>316</v>
       </c>
       <c r="D137" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="E137" t="s">
-        <v>100</v>
+        <v>316</v>
       </c>
       <c r="F137" t="s">
-        <v>201</v>
+        <v>316</v>
       </c>
       <c r="G137" t="s">
-        <v>225</v>
+        <v>316</v>
       </c>
       <c r="H137" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="I137" t="s">
-        <v>99</v>
+        <v>316</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B138" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C138" t="s">
         <v>27</v>
@@ -5328,10 +5334,10 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>258</v>
+        <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>262</v>
+        <v>90</v>
       </c>
       <c r="C139" t="s">
         <v>27</v>
@@ -5357,10 +5363,10 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B140" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C140" t="s">
         <v>27</v>
@@ -5386,10 +5392,10 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B141" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C141" t="s">
         <v>27</v>
@@ -5415,10 +5421,10 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B142" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C142" t="s">
         <v>27</v>
@@ -5443,29 +5449,32 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>261</v>
+      </c>
       <c r="B143" t="s">
-        <v>316</v>
+        <v>265</v>
       </c>
       <c r="C143" t="s">
-        <v>316</v>
+        <v>27</v>
       </c>
       <c r="D143" t="s">
-        <v>316</v>
+        <v>24</v>
       </c>
       <c r="E143" t="s">
-        <v>316</v>
+        <v>100</v>
       </c>
       <c r="F143" t="s">
-        <v>316</v>
+        <v>201</v>
       </c>
       <c r="G143" t="s">
-        <v>316</v>
+        <v>225</v>
       </c>
       <c r="H143" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="I143" t="s">
-        <v>316</v>
+        <v>99</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -5495,9 +5504,6 @@
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>313</v>
-      </c>
       <c r="B145" t="s">
         <v>316</v>
       </c>
@@ -5525,28 +5531,28 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>17</v>
+        <v>313</v>
       </c>
       <c r="B146" t="s">
-        <v>34</v>
+        <v>316</v>
       </c>
       <c r="C146" t="s">
-        <v>27</v>
+        <v>316</v>
       </c>
       <c r="D146" t="s">
-        <v>24</v>
+        <v>316</v>
       </c>
       <c r="E146" t="s">
         <v>316</v>
       </c>
       <c r="F146" t="s">
-        <v>226</v>
+        <v>316</v>
       </c>
       <c r="G146" t="s">
-        <v>215</v>
+        <v>316</v>
       </c>
       <c r="H146" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I146" t="s">
         <v>316</v>
@@ -5554,10 +5560,10 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B147" t="s">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="C147" t="s">
         <v>27</v>
@@ -5566,10 +5572,10 @@
         <v>24</v>
       </c>
       <c r="E147" t="s">
-        <v>124</v>
+        <v>316</v>
       </c>
       <c r="F147" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="G147" t="s">
         <v>215</v>
@@ -5583,10 +5589,10 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>216</v>
+        <v>0</v>
       </c>
       <c r="B148" t="s">
-        <v>217</v>
+        <v>130</v>
       </c>
       <c r="C148" t="s">
         <v>27</v>
@@ -5612,10 +5618,10 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>1</v>
+        <v>216</v>
       </c>
       <c r="B149" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="C149" t="s">
         <v>27</v>
@@ -5641,10 +5647,10 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="B150" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C150" t="s">
         <v>27</v>
@@ -5653,13 +5659,13 @@
         <v>24</v>
       </c>
       <c r="E150" t="s">
-        <v>316</v>
+        <v>124</v>
       </c>
       <c r="F150" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="G150" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="H150" t="s">
         <v>322</v>
@@ -5670,10 +5676,10 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>335</v>
+        <v>131</v>
       </c>
       <c r="B151" t="s">
-        <v>336</v>
+        <v>133</v>
       </c>
       <c r="C151" t="s">
         <v>27</v>
@@ -5681,37 +5687,40 @@
       <c r="D151" t="s">
         <v>24</v>
       </c>
+      <c r="E151" t="s">
+        <v>316</v>
+      </c>
       <c r="F151" t="s">
+        <v>210</v>
+      </c>
+      <c r="G151" t="s">
+        <v>225</v>
+      </c>
+      <c r="H151" t="s">
+        <v>322</v>
+      </c>
+      <c r="I151" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>335</v>
+      </c>
+      <c r="B152" t="s">
+        <v>336</v>
+      </c>
+      <c r="C152" t="s">
+        <v>27</v>
+      </c>
+      <c r="D152" t="s">
+        <v>24</v>
+      </c>
+      <c r="F152" t="s">
         <v>202</v>
       </c>
-      <c r="H151" t="s">
+      <c r="H152" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B152" t="s">
-        <v>316</v>
-      </c>
-      <c r="C152" t="s">
-        <v>316</v>
-      </c>
-      <c r="D152" t="s">
-        <v>316</v>
-      </c>
-      <c r="E152" t="s">
-        <v>316</v>
-      </c>
-      <c r="F152" t="s">
-        <v>316</v>
-      </c>
-      <c r="G152" t="s">
-        <v>316</v>
-      </c>
-      <c r="H152" t="s">
-        <v>316</v>
-      </c>
-      <c r="I152" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5741,9 +5750,6 @@
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>314</v>
-      </c>
       <c r="B154" t="s">
         <v>316</v>
       </c>
@@ -5771,28 +5777,28 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="B155" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="C155" t="s">
-        <v>27</v>
+        <v>316</v>
       </c>
       <c r="D155" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="E155" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="F155" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="G155" t="s">
-        <v>225</v>
+        <v>316</v>
       </c>
       <c r="H155" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="I155" t="s">
         <v>316</v>
@@ -5800,10 +5806,10 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B156" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C156" t="s">
         <v>27</v>
@@ -5829,10 +5835,10 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B157" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C157" t="s">
         <v>27</v>
@@ -5858,10 +5864,10 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B158" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C158" t="s">
         <v>27</v>
@@ -5887,16 +5893,16 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B159" t="s">
-        <v>122</v>
+        <v>296</v>
       </c>
       <c r="C159" t="s">
         <v>27</v>
       </c>
       <c r="D159" t="s">
-        <v>166</v>
+        <v>292</v>
       </c>
       <c r="E159" t="s">
         <v>293</v>
@@ -5916,7 +5922,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>46</v>
+        <v>282</v>
       </c>
       <c r="B160" t="s">
         <v>122</v>
@@ -5928,7 +5934,7 @@
         <v>166</v>
       </c>
       <c r="E160" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F160" t="s">
         <v>293</v>
@@ -5945,7 +5951,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>283</v>
+        <v>46</v>
       </c>
       <c r="B161" t="s">
         <v>122</v>
@@ -5954,10 +5960,10 @@
         <v>27</v>
       </c>
       <c r="D161" t="s">
-        <v>292</v>
+        <v>166</v>
       </c>
       <c r="E161" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="F161" t="s">
         <v>293</v>
@@ -5974,7 +5980,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B162" t="s">
         <v>122</v>
@@ -5986,7 +5992,7 @@
         <v>292</v>
       </c>
       <c r="E162" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F162" t="s">
         <v>293</v>
@@ -6003,28 +6009,28 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B163" t="s">
         <v>122</v>
       </c>
       <c r="C163" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D163" t="s">
-        <v>25</v>
+        <v>292</v>
       </c>
       <c r="E163" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="F163" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="G163" t="s">
-        <v>25</v>
+        <v>225</v>
       </c>
       <c r="H163" t="s">
-        <v>25</v>
+        <v>325</v>
       </c>
       <c r="I163" t="s">
         <v>316</v>
@@ -6032,28 +6038,28 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B164" t="s">
         <v>122</v>
       </c>
       <c r="C164" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D164" t="s">
-        <v>292</v>
+        <v>25</v>
       </c>
       <c r="E164" t="s">
-        <v>123</v>
+        <v>316</v>
       </c>
       <c r="F164" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="G164" t="s">
-        <v>225</v>
+        <v>25</v>
       </c>
       <c r="H164" t="s">
-        <v>325</v>
+        <v>25</v>
       </c>
       <c r="I164" t="s">
         <v>316</v>
@@ -6061,7 +6067,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B165" t="s">
         <v>122</v>
@@ -6090,7 +6096,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B166" t="s">
         <v>122</v>
@@ -6119,7 +6125,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B167" t="s">
         <v>122</v>
@@ -6148,7 +6154,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B168" t="s">
         <v>122</v>
@@ -6175,36 +6181,36 @@
         <v>316</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
-        <v>316</v>
-      </c>
-      <c r="C170" t="s">
-        <v>316</v>
-      </c>
-      <c r="D170" t="s">
-        <v>316</v>
-      </c>
-      <c r="E170" t="s">
-        <v>316</v>
-      </c>
-      <c r="F170" t="s">
-        <v>316</v>
-      </c>
-      <c r="G170" t="s">
-        <v>316</v>
-      </c>
-      <c r="H170" t="s">
-        <v>316</v>
-      </c>
-      <c r="I170" t="s">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>290</v>
+      </c>
+      <c r="B169" t="s">
+        <v>122</v>
+      </c>
+      <c r="C169" t="s">
+        <v>27</v>
+      </c>
+      <c r="D169" t="s">
+        <v>292</v>
+      </c>
+      <c r="E169" t="s">
+        <v>123</v>
+      </c>
+      <c r="F169" t="s">
+        <v>293</v>
+      </c>
+      <c r="G169" t="s">
+        <v>225</v>
+      </c>
+      <c r="H169" t="s">
+        <v>325</v>
+      </c>
+      <c r="I169" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>315</v>
-      </c>
       <c r="B171" t="s">
         <v>316</v>
       </c>
@@ -6232,28 +6238,28 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>251</v>
+        <v>315</v>
       </c>
       <c r="B172" t="s">
-        <v>252</v>
+        <v>316</v>
       </c>
       <c r="C172" t="s">
-        <v>27</v>
+        <v>316</v>
       </c>
       <c r="D172" t="s">
-        <v>166</v>
+        <v>316</v>
       </c>
       <c r="E172" t="s">
-        <v>115</v>
+        <v>316</v>
       </c>
       <c r="F172" t="s">
-        <v>199</v>
+        <v>316</v>
       </c>
       <c r="G172" t="s">
-        <v>225</v>
+        <v>316</v>
       </c>
       <c r="H172" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="I172" t="s">
         <v>316</v>
@@ -6261,10 +6267,10 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>80</v>
+        <v>251</v>
       </c>
       <c r="B173" t="s">
-        <v>114</v>
+        <v>252</v>
       </c>
       <c r="C173" t="s">
         <v>27</v>
@@ -6290,10 +6296,10 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>253</v>
+        <v>80</v>
       </c>
       <c r="B174" t="s">
-        <v>254</v>
+        <v>114</v>
       </c>
       <c r="C174" t="s">
         <v>27</v>
@@ -6319,10 +6325,10 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>81</v>
+        <v>253</v>
       </c>
       <c r="B175" t="s">
-        <v>158</v>
+        <v>254</v>
       </c>
       <c r="C175" t="s">
         <v>27</v>
@@ -6331,10 +6337,10 @@
         <v>166</v>
       </c>
       <c r="E175" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
       <c r="F175" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G175" t="s">
         <v>225</v>
@@ -6346,14 +6352,43 @@
         <v>316</v>
       </c>
     </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>81</v>
+      </c>
+      <c r="B176" t="s">
+        <v>158</v>
+      </c>
+      <c r="C176" t="s">
+        <v>27</v>
+      </c>
+      <c r="D176" t="s">
+        <v>166</v>
+      </c>
+      <c r="E176" t="s">
+        <v>159</v>
+      </c>
+      <c r="F176" t="s">
+        <v>208</v>
+      </c>
+      <c r="G176" t="s">
+        <v>225</v>
+      </c>
+      <c r="H176" t="s">
+        <v>326</v>
+      </c>
+      <c r="I176" t="s">
+        <v>316</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:I175" xr:uid="{6ACFB32A-97A1-4D27-B533-EB469205C671}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I130">
-      <sortCondition ref="D2:D130"/>
+  <autoFilter ref="A2:I176" xr:uid="{6ACFB32A-97A1-4D27-B533-EB469205C671}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I131">
+      <sortCondition ref="D2:D131"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I130">
-    <sortCondition ref="A3:A130"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I131">
+    <sortCondition ref="A3:A131"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>